<commit_message>
door quote generator notes added
</commit_message>
<xml_diff>
--- a/notes - something.pk.xlsx
+++ b/notes - something.pk.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>v 0.1</t>
   </si>
@@ -71,90 +71,52 @@
     <t>United Bank Limited</t>
   </si>
   <si>
-    <t xml:space="preserve">Purpose: </t>
-  </si>
-  <si>
-    <t>easily food ordering mechanism for 36 galas, 50 thaals per gala</t>
-  </si>
-  <si>
     <t>Use Cases</t>
   </si>
   <si>
-    <t>add menu for the day</t>
-  </si>
-  <si>
     <t>S/N</t>
   </si>
   <si>
-    <t>start stop food sessions In progress, (breakfast, lunch, dinner)</t>
-  </si>
-  <si>
-    <t>select gala to manage</t>
-  </si>
-  <si>
-    <t>add captains, assign galas to captains</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">user types: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>admin, kitchen supervisor, gala supervisor</t>
-    </r>
-  </si>
-  <si>
-    <t>Brain Storm</t>
-  </si>
-  <si>
-    <t>admin: dispatch order</t>
-  </si>
-  <si>
-    <t>gala: request order for item</t>
-  </si>
-  <si>
-    <t>admin: see all pending request orders</t>
-  </si>
-  <si>
-    <t>gala: see all pending requests</t>
-  </si>
-  <si>
-    <t>gala: confirm request order received</t>
-  </si>
-  <si>
-    <t>admin: see old the request order is pending</t>
-  </si>
-  <si>
-    <t>gala: return unused food???</t>
-  </si>
-  <si>
-    <t>app designed for 320px width, android, chrome browser</t>
-  </si>
-  <si>
     <t>make the system so good that they are forced to use it even after Moharram</t>
   </si>
   <si>
-    <t>admin: create new day with new food menu</t>
-  </si>
-  <si>
-    <t>create and print list of galas and passwords, instead of using emails</t>
-  </si>
-  <si>
-    <t>set name with each gala</t>
+    <t>MVP for door quotes and manufacturing</t>
+  </si>
+  <si>
+    <t>APP:</t>
+  </si>
+  <si>
+    <t>Visitor work flow</t>
+  </si>
+  <si>
+    <t>select fire rating</t>
+  </si>
+  <si>
+    <t>specify size</t>
+  </si>
+  <si>
+    <t>add comments</t>
+  </si>
+  <si>
+    <t>generate comments</t>
+  </si>
+  <si>
+    <t>get quote</t>
+  </si>
+  <si>
+    <t>get email for a new quote</t>
+  </si>
+  <si>
+    <t>add special requirements</t>
+  </si>
+  <si>
+    <t>Input Company Name , Address, Email, Project Name:</t>
+  </si>
+  <si>
+    <t>approve quote in email</t>
+  </si>
+  <si>
+    <t>quote is automatically generated and sent to the client</t>
   </si>
 </sst>
 </file>
@@ -224,13 +186,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,21 +274,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -810,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I21"/>
+  <dimension ref="B1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:G20"/>
+      <selection activeCell="C16" sqref="C16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,263 +786,283 @@
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+    </row>
+    <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="I5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
         <v>3</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="16">
         <v>4</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-    </row>
-    <row r="8" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="I7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+    </row>
+    <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
         <v>5</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="I8" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="I9" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <v>7</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
-        <v>8</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="29">
-        <v>9</v>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
-        <v>10</v>
-      </c>
-      <c r="C13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>2</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
-        <v>11</v>
-      </c>
-      <c r="C14" s="32" t="s">
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>3</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
-        <v>12</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
-        <v>13</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+        <v>4</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
-        <v>14</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
+        <v>5</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="29">
-        <v>15</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
+      <c r="B18" s="24">
+        <v>6</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
-        <v>16</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
+        <v>7</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
+  <mergeCells count="25">
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="I9:M9"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="C4:G4"/>
@@ -1089,6 +1071,18 @@
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>